<commit_message>
Fix date format in report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DOCTOLIBSRLXX/Doctolib/Vettore/26/report-checklist.xlsx
+++ b/GATEWAY/A1#111DOCTOLIBSRLXX/Doctolib/Vettore/26/report-checklist.xlsx
@@ -20,7 +20,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -4270,10 +4270,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -4491,7 +4492,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4634,6 +4635,10 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -4956,7 +4961,7 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6030,7 +6035,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -7139,7 +7144,7 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -7703,7 +7708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="24.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25" t="n">
         <v>11</v>
       </c>
@@ -7741,7 +7746,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="24.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="n">
         <v>12</v>
       </c>
@@ -7779,7 +7784,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="n">
         <v>13</v>
       </c>
@@ -7817,7 +7822,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="24.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="n">
         <v>14</v>
       </c>
@@ -8365,7 +8370,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="69.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25" t="n">
         <v>31</v>
       </c>
@@ -8403,7 +8408,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="69.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="25" t="n">
         <v>32</v>
       </c>
@@ -8645,7 +8650,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="69.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="25" t="n">
         <v>39</v>
       </c>
@@ -8683,7 +8688,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="69.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="25" t="n">
         <v>40</v>
       </c>
@@ -8979,7 +8984,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="46.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="25" t="n">
         <v>48</v>
       </c>
@@ -9917,7 +9922,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="102.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="25" t="n">
         <v>75</v>
       </c>
@@ -9955,7 +9960,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="25" t="n">
         <v>76</v>
       </c>
@@ -9993,7 +9998,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="25" t="n">
         <v>77</v>
       </c>
@@ -10031,7 +10036,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="25" t="n">
         <v>78</v>
       </c>
@@ -10069,7 +10074,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="25" t="n">
         <v>79</v>
       </c>
@@ -10107,7 +10112,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="25" t="n">
         <v>80</v>
       </c>
@@ -10145,7 +10150,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="25" t="n">
         <v>81</v>
       </c>
@@ -10183,7 +10188,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="25" t="n">
         <v>82</v>
       </c>
@@ -10221,7 +10226,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="25" t="n">
         <v>83</v>
       </c>
@@ -10259,7 +10264,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="25" t="n">
         <v>84</v>
       </c>
@@ -10297,7 +10302,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="25" t="n">
         <v>85</v>
       </c>
@@ -10335,7 +10340,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="25" t="n">
         <v>86</v>
       </c>
@@ -10373,7 +10378,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="102.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="25" t="n">
         <v>87</v>
       </c>
@@ -10411,7 +10416,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="25" t="n">
         <v>88</v>
       </c>
@@ -10449,7 +10454,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="25" t="n">
         <v>89</v>
       </c>
@@ -10487,7 +10492,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="25" t="n">
         <v>90</v>
       </c>
@@ -10525,7 +10530,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="25" t="n">
         <v>91</v>
       </c>
@@ -10563,7 +10568,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="25" t="n">
         <v>92</v>
       </c>
@@ -10601,7 +10606,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="25" t="n">
         <v>93</v>
       </c>
@@ -12441,7 +12446,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="124.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="124.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="25" t="n">
         <v>147</v>
       </c>
@@ -12479,7 +12484,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="124.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="124.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="25" t="n">
         <v>148</v>
       </c>
@@ -12517,7 +12522,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="124.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="124.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="25" t="n">
         <v>149</v>
       </c>
@@ -12555,7 +12560,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="124.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="124.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="25" t="n">
         <v>150</v>
       </c>
@@ -12571,7 +12576,7 @@
       <c r="E157" s="27" t="s">
         <v>356</v>
       </c>
-      <c r="F157" s="28"/>
+      <c r="F157" s="36"/>
       <c r="G157" s="29"/>
       <c r="H157" s="29"/>
       <c r="I157" s="29"/>
@@ -12593,7 +12598,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="25" t="n">
         <v>151</v>
       </c>
@@ -12631,7 +12636,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="25" t="n">
         <v>152</v>
       </c>
@@ -12669,7 +12674,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="25" t="n">
         <v>153</v>
       </c>
@@ -12707,7 +12712,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="25" t="n">
         <v>154</v>
       </c>
@@ -12745,7 +12750,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="25" t="n">
         <v>155</v>
       </c>
@@ -12783,7 +12788,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="25" t="n">
         <v>156</v>
       </c>
@@ -12821,7 +12826,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="25" t="n">
         <v>157</v>
       </c>
@@ -12859,7 +12864,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="25" t="n">
         <v>158</v>
       </c>
@@ -12897,7 +12902,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="25" t="n">
         <v>159</v>
       </c>
@@ -12935,7 +12940,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="25" t="n">
         <v>160</v>
       </c>
@@ -12973,7 +12978,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="25" t="n">
         <v>161</v>
       </c>
@@ -13011,7 +13016,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="25" t="n">
         <v>162</v>
       </c>
@@ -13049,7 +13054,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="25" t="n">
         <v>163</v>
       </c>
@@ -13087,7 +13092,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="25" t="n">
         <v>164</v>
       </c>
@@ -13125,7 +13130,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="25" t="n">
         <v>165</v>
       </c>
@@ -13163,7 +13168,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="25" t="n">
         <v>166</v>
       </c>
@@ -13201,7 +13206,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="25" t="n">
         <v>167</v>
       </c>
@@ -13239,7 +13244,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="25" t="n">
         <v>168</v>
       </c>
@@ -13277,7 +13282,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="25" t="n">
         <v>169</v>
       </c>
@@ -15168,7 +15173,7 @@
         <v>512</v>
       </c>
       <c r="F231" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G231" s="29" t="s">
         <v>513</v>
@@ -15195,7 +15200,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="192.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="191.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="25" t="n">
         <v>225</v>
       </c>
@@ -15212,7 +15217,7 @@
         <v>517</v>
       </c>
       <c r="F232" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G232" s="29" t="s">
         <v>518</v>
@@ -15239,7 +15244,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="178.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="25" t="n">
         <v>226</v>
       </c>
@@ -15256,7 +15261,7 @@
         <v>522</v>
       </c>
       <c r="F233" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G233" s="29" t="s">
         <v>523</v>
@@ -15283,7 +15288,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="107.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="25" t="n">
         <v>227</v>
       </c>
@@ -15300,7 +15305,7 @@
         <v>527</v>
       </c>
       <c r="F234" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G234" s="29" t="s">
         <v>528</v>
@@ -15327,7 +15332,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="180.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="25" t="n">
         <v>228</v>
       </c>
@@ -15344,7 +15349,7 @@
         <v>532</v>
       </c>
       <c r="F235" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G235" s="29" t="s">
         <v>533</v>
@@ -15371,7 +15376,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="136.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="135.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="25" t="n">
         <v>229</v>
       </c>
@@ -15388,7 +15393,7 @@
         <v>537</v>
       </c>
       <c r="F236" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G236" s="29" t="s">
         <v>538</v>
@@ -15413,7 +15418,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="136.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="136.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="25" t="n">
         <v>230</v>
       </c>
@@ -15451,7 +15456,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="166.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="25" t="n">
         <v>231</v>
       </c>
@@ -15468,7 +15473,7 @@
         <v>544</v>
       </c>
       <c r="F238" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G238" s="29" t="s">
         <v>545</v>
@@ -15495,7 +15500,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="147.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="147.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="25" t="n">
         <v>232</v>
       </c>
@@ -15533,7 +15538,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="136.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="136.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="25" t="n">
         <v>233</v>
       </c>
@@ -15571,7 +15576,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="147.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="147.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="25" t="n">
         <v>234</v>
       </c>
@@ -15609,7 +15614,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="25" t="n">
         <v>235</v>
       </c>
@@ -15647,7 +15652,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="95.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="25" t="n">
         <v>236</v>
       </c>
@@ -15664,7 +15669,7 @@
         <v>473</v>
       </c>
       <c r="F243" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G243" s="29" t="s">
         <v>558</v>
@@ -15689,7 +15694,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="166.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="25" t="n">
         <v>237</v>
       </c>
@@ -15706,7 +15711,7 @@
         <v>561</v>
       </c>
       <c r="F244" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G244" s="29" t="s">
         <v>562</v>
@@ -15731,7 +15736,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="178.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="25" t="n">
         <v>238</v>
       </c>
@@ -15748,7 +15753,7 @@
         <v>565</v>
       </c>
       <c r="F245" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G245" s="29" t="s">
         <v>566</v>
@@ -15790,7 +15795,7 @@
         <v>569</v>
       </c>
       <c r="F246" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G246" s="29" t="s">
         <v>570</v>
@@ -17447,7 +17452,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="124.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="131.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="25" t="n">
         <v>288</v>
       </c>
@@ -17464,7 +17469,7 @@
         <v>666</v>
       </c>
       <c r="F295" s="28" t="n">
-        <v>45508</v>
+        <v>45390</v>
       </c>
       <c r="G295" s="29" t="s">
         <v>667</v>
@@ -17491,7 +17496,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="192.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="191.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="25" t="n">
         <v>289</v>
       </c>
@@ -17508,7 +17513,7 @@
         <v>671</v>
       </c>
       <c r="F296" s="28" t="n">
-        <v>45508</v>
+        <v>45390</v>
       </c>
       <c r="G296" s="29" t="s">
         <v>672</v>
@@ -17535,7 +17540,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="178.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="25" t="n">
         <v>290</v>
       </c>
@@ -17552,7 +17557,7 @@
         <v>676</v>
       </c>
       <c r="F297" s="28" t="n">
-        <v>45508</v>
+        <v>45390</v>
       </c>
       <c r="G297" s="29" t="s">
         <v>677</v>
@@ -17579,7 +17584,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="102.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="107.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="25" t="n">
         <v>291</v>
       </c>
@@ -17596,7 +17601,7 @@
         <v>681</v>
       </c>
       <c r="F298" s="28" t="n">
-        <v>45508</v>
+        <v>45390</v>
       </c>
       <c r="G298" s="29" t="s">
         <v>682</v>
@@ -17623,7 +17628,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="180.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="180.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="25" t="n">
         <v>292</v>
       </c>
@@ -17640,7 +17645,7 @@
         <v>686</v>
       </c>
       <c r="F299" s="28" t="n">
-        <v>45508</v>
+        <v>45390</v>
       </c>
       <c r="G299" s="29" t="s">
         <v>687</v>
@@ -17667,7 +17672,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="25" t="n">
         <v>293</v>
       </c>
@@ -17684,7 +17689,7 @@
         <v>691</v>
       </c>
       <c r="F300" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G300" s="29" t="s">
         <v>692</v>
@@ -17709,7 +17714,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="136.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="136.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="25" t="n">
         <v>294</v>
       </c>
@@ -17747,7 +17752,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="166.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="25" t="n">
         <v>295</v>
       </c>
@@ -17764,7 +17769,7 @@
         <v>697</v>
       </c>
       <c r="F302" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G302" s="29" t="s">
         <v>698</v>
@@ -17791,7 +17796,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="147.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="147.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="25" t="n">
         <v>296</v>
       </c>
@@ -17829,7 +17834,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="136.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="136.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="25" t="n">
         <v>297</v>
       </c>
@@ -17867,7 +17872,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="147.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="147.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="25" t="n">
         <v>298</v>
       </c>
@@ -17905,7 +17910,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="25" t="n">
         <v>299</v>
       </c>
@@ -17943,7 +17948,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="91.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="95.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="25" t="n">
         <v>300</v>
       </c>
@@ -17960,7 +17965,7 @@
         <v>473</v>
       </c>
       <c r="F307" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G307" s="29" t="s">
         <v>710</v>
@@ -17985,7 +17990,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="166.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="25" t="n">
         <v>301</v>
       </c>
@@ -18002,7 +18007,7 @@
         <v>713</v>
       </c>
       <c r="F308" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G308" s="29" t="s">
         <v>714</v>
@@ -18027,7 +18032,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="178.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="25" t="n">
         <v>302</v>
       </c>
@@ -18044,7 +18049,7 @@
         <v>717</v>
       </c>
       <c r="F309" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G309" s="29" t="s">
         <v>718</v>
@@ -18069,7 +18074,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="25" t="n">
         <v>303</v>
       </c>
@@ -18086,7 +18091,7 @@
         <v>721</v>
       </c>
       <c r="F310" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G310" s="29" t="s">
         <v>722</v>
@@ -18927,7 +18932,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="192.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="192.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="25" t="n">
         <v>328</v>
       </c>
@@ -18965,7 +18970,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="25" t="n">
         <v>329</v>
       </c>
@@ -19003,7 +19008,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="180.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="180.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="25" t="n">
         <v>330</v>
       </c>
@@ -19041,7 +19046,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="25" t="n">
         <v>331</v>
       </c>
@@ -19487,7 +19492,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="192.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="192.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="25" t="n">
         <v>344</v>
       </c>
@@ -19525,7 +19530,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="25" t="n">
         <v>345</v>
       </c>
@@ -19563,7 +19568,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="353" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="25" t="n">
         <v>346</v>
       </c>
@@ -19601,7 +19606,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="354" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="25" t="n">
         <v>347</v>
       </c>
@@ -19911,7 +19916,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="180.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="180.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="25" t="n">
         <v>356</v>
       </c>
@@ -19949,7 +19954,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="25" t="n">
         <v>357</v>
       </c>
@@ -20191,7 +20196,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="371" customFormat="false" ht="180.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" customFormat="false" ht="180.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="25" t="n">
         <v>364</v>
       </c>
@@ -20229,7 +20234,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="372" customFormat="false" ht="158.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" customFormat="false" ht="158.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="25" t="n">
         <v>365</v>
       </c>
@@ -20403,7 +20408,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="377" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="377" customFormat="false" ht="107.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="25" t="n">
         <v>370</v>
       </c>
@@ -20420,7 +20425,7 @@
         <v>858</v>
       </c>
       <c r="F377" s="28" t="n">
-        <v>45539</v>
+        <v>45391</v>
       </c>
       <c r="G377" s="29" t="s">
         <v>859</v>
@@ -20549,7 +20554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="381" customFormat="false" ht="57.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" customFormat="false" ht="124.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="25" t="n">
         <v>374</v>
       </c>
@@ -20566,7 +20571,7 @@
         <v>869</v>
       </c>
       <c r="F381" s="28" t="n">
-        <v>45508</v>
+        <v>45390</v>
       </c>
       <c r="G381" s="29" t="s">
         <v>870</v>
@@ -25314,14 +25319,15 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T383">
-    <filterColumn colId="9">
-      <filters blank="1">
-        <filter val="SI"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="RAD"/>
+        <filter val="RSA"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters blank="1">
+        <dateGroupItem year="2024" month="04" day="09" dateTimeGrouping="day"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -25345,7 +25351,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E235" r:id="rId2" display="https://github.com"/>
+    <hyperlink ref="E235" r:id="rId2" display="Prerequisito: si esegue con esito positivo il caso di test PUBBLICAZIONE_CREAZIONE_CDA2_RAD_CT1&#10;&#10;Viene richiamato il servizio di Aggiornamento Metadati &quot;https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/&lt;idDoc&gt;/metadata&quot;al fine di testare l'aggiornamento dei metadati (&quot;attiCliniciRegoleAccesso&quot;), in particolare l'oscuramento di un documento CDA2  precedentemente pubblicato. La corretta valorizzazione dei metadati comporterà un esito positivo (status code 200), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.&#10;&#10;Per la richiesta è necessario:&#10;▪per l'utente che è in grado di procedere in autonomia, comporre i metadati della RequestBody conformemente a quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway;&#10;▪per l'utente che non è in grado di procedere in autonomia, comporre i metadati contenente la RequestBody utilizzando il json &quot;RAD - Caso di Test 4 - Oscuramento&quot; presente al path &quot;https://github.com/ministero-salute/it-fse-accreditamento&quot;.&#10;&#10;Per tutti gli utenti è necessario che il campo &quot;idDoc&quot;da passare nell'endpoint sia valorizzato con l'identificativo del documento precedentemente pubblicato (caso di test PUBBLICAZIONE_CREAZIONE_CDA2_RAD_CT1)."/>
     <hyperlink ref="E300" r:id="rId3" display="Prerequisito: per i fornitori in grado di validare, non deve essere effettuata la validazione del documento da pubblicare.&#10;&#10;Viene richiamato il servizio di pubblicazione &quot;https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents&quot; al fine di testare la pubblicazione creazione con esito KO (status code 400) di un documento non validato, con la corretta valorizzazione dei metadati, secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.&#10;&#10;Per la richiesta, se il fornitore non ha la possibilità di avere a disposizione un documento, è possibile:&#10;▪utilizzare il documento &quot;SIGNED_RSA1.pdf&quot; presente al path https://github.com/ministero-salute/it-fse-accreditamento; &#10;▪comporre i metadati contenente la RequestBody utilizzando il json &quot;RSA - Caso di Test 4 - Create&quot; presente al path &quot;https://github.com/ministero-salute/it-fse-accreditamento&quot;.&#10;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -25367,7 +25373,7 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
@@ -25403,10 +25409,10 @@
       <c r="B2" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>880</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>881</v>
       </c>
     </row>
@@ -25417,10 +25423,10 @@
       <c r="B3" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>882</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="37" t="s">
         <v>883</v>
       </c>
     </row>
@@ -25431,10 +25437,10 @@
       <c r="B4" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>884</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="38" t="s">
         <v>885</v>
       </c>
     </row>
@@ -25445,10 +25451,10 @@
       <c r="B5" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>886</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="37" t="s">
         <v>887</v>
       </c>
     </row>
@@ -25459,10 +25465,10 @@
       <c r="B6" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>888</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="38" t="s">
         <v>889</v>
       </c>
     </row>
@@ -25473,10 +25479,10 @@
       <c r="B7" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="37" t="s">
         <v>890</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="38" t="s">
         <v>891</v>
       </c>
     </row>
@@ -25487,10 +25493,10 @@
       <c r="B8" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>892</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>893</v>
       </c>
     </row>
@@ -25501,10 +25507,10 @@
       <c r="B9" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="37" t="s">
         <v>894</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="38" t="s">
         <v>895</v>
       </c>
     </row>
@@ -25515,10 +25521,10 @@
       <c r="B10" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="38" t="s">
         <v>897</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="37" t="s">
         <v>898</v>
       </c>
     </row>
@@ -25529,10 +25535,10 @@
       <c r="B11" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C11" s="36" t="n">
+      <c r="C11" s="37" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="37" t="s">
         <v>900</v>
       </c>
     </row>
@@ -25543,10 +25549,10 @@
       <c r="B12" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C12" s="36" t="n">
+      <c r="C12" s="37" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="37" t="s">
         <v>901</v>
       </c>
     </row>
@@ -25557,10 +25563,10 @@
       <c r="B13" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C13" s="36" t="n">
+      <c r="C13" s="37" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="38" t="s">
         <v>902</v>
       </c>
     </row>
@@ -25571,10 +25577,10 @@
       <c r="B14" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C14" s="36" t="n">
+      <c r="C14" s="37" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="37" t="s">
         <v>903</v>
       </c>
     </row>
@@ -25585,10 +25591,10 @@
       <c r="B15" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C15" s="36" t="n">
+      <c r="C15" s="37" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="38" t="s">
         <v>904</v>
       </c>
     </row>
@@ -25599,10 +25605,10 @@
       <c r="B16" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C16" s="36" t="n">
+      <c r="C16" s="37" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="38" t="s">
         <v>905</v>
       </c>
     </row>
@@ -25613,10 +25619,10 @@
       <c r="B17" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C17" s="36" t="n">
+      <c r="C17" s="37" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="38" t="s">
         <v>906</v>
       </c>
     </row>
@@ -25627,10 +25633,10 @@
       <c r="B18" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="C18" s="36" t="n">
+      <c r="C18" s="37" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="38" t="s">
         <v>907</v>
       </c>
     </row>
@@ -25641,10 +25647,10 @@
       <c r="B19" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C19" s="36" t="n">
+      <c r="C19" s="37" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="37" t="s">
         <v>909</v>
       </c>
     </row>
@@ -25655,10 +25661,10 @@
       <c r="B20" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C20" s="36" t="n">
+      <c r="C20" s="37" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="37" t="s">
         <v>910</v>
       </c>
     </row>
@@ -25669,10 +25675,10 @@
       <c r="B21" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C21" s="36" t="n">
+      <c r="C21" s="37" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="38" t="s">
         <v>911</v>
       </c>
     </row>
@@ -25683,10 +25689,10 @@
       <c r="B22" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C22" s="36" t="n">
+      <c r="C22" s="37" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="37" t="s">
         <v>912</v>
       </c>
     </row>
@@ -25697,10 +25703,10 @@
       <c r="B23" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C23" s="36" t="n">
+      <c r="C23" s="37" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="38" t="s">
         <v>913</v>
       </c>
     </row>
@@ -25711,10 +25717,10 @@
       <c r="B24" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C24" s="36" t="n">
+      <c r="C24" s="37" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="38" t="s">
         <v>914</v>
       </c>
     </row>
@@ -25725,10 +25731,10 @@
       <c r="B25" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C25" s="36" t="n">
+      <c r="C25" s="37" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="38" t="s">
         <v>915</v>
       </c>
     </row>
@@ -25739,10 +25745,10 @@
       <c r="B26" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C26" s="36" t="n">
+      <c r="C26" s="37" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="38" t="s">
         <v>916</v>
       </c>
     </row>
@@ -25753,10 +25759,10 @@
       <c r="B27" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C27" s="36" t="n">
+      <c r="C27" s="37" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="37" t="s">
         <v>918</v>
       </c>
     </row>
@@ -25767,10 +25773,10 @@
       <c r="B28" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C28" s="36" t="n">
+      <c r="C28" s="37" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="37" t="s">
         <v>919</v>
       </c>
     </row>
@@ -25781,10 +25787,10 @@
       <c r="B29" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C29" s="36" t="n">
+      <c r="C29" s="37" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="39" t="s">
         <v>920</v>
       </c>
     </row>
@@ -25795,10 +25801,10 @@
       <c r="B30" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C30" s="36" t="n">
+      <c r="C30" s="37" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D30" s="37" t="s">
         <v>921</v>
       </c>
     </row>
@@ -25809,10 +25815,10 @@
       <c r="B31" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C31" s="36" t="n">
+      <c r="C31" s="37" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="38" t="s">
         <v>922</v>
       </c>
     </row>
@@ -25823,10 +25829,10 @@
       <c r="B32" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C32" s="36" t="n">
+      <c r="C32" s="37" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="38" t="s">
         <v>923</v>
       </c>
     </row>
@@ -25837,10 +25843,10 @@
       <c r="B33" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C33" s="36" t="n">
+      <c r="C33" s="37" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="38" t="s">
         <v>924</v>
       </c>
     </row>
@@ -25851,10 +25857,10 @@
       <c r="B34" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="C34" s="36" t="n">
+      <c r="C34" s="37" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="37" t="s">
+      <c r="D34" s="38" t="s">
         <v>925</v>
       </c>
     </row>
@@ -25865,10 +25871,10 @@
       <c r="B35" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="C35" s="36" t="n">
+      <c r="C35" s="37" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="36" t="n">
+      <c r="D35" s="37" t="n">
         <v>204</v>
       </c>
     </row>
@@ -25879,10 +25885,10 @@
       <c r="B36" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="C36" s="36" t="n">
+      <c r="C36" s="37" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="36" t="n">
+      <c r="D36" s="37" t="n">
         <v>220</v>
       </c>
     </row>
@@ -25893,10 +25899,10 @@
       <c r="B37" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="C37" s="36" t="n">
+      <c r="C37" s="37" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="37" t="n">
+      <c r="D37" s="38" t="n">
         <v>236</v>
       </c>
     </row>
@@ -25907,10 +25913,10 @@
       <c r="B38" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="C38" s="36" t="n">
+      <c r="C38" s="37" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="36" t="n">
+      <c r="D38" s="37" t="n">
         <v>252</v>
       </c>
     </row>
@@ -25921,10 +25927,10 @@
       <c r="B39" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="C39" s="36" t="n">
+      <c r="C39" s="37" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="37" t="n">
+      <c r="D39" s="38" t="n">
         <v>268</v>
       </c>
     </row>
@@ -25935,10 +25941,10 @@
       <c r="B40" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="C40" s="36" t="n">
+      <c r="C40" s="37" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="37" t="n">
+      <c r="D40" s="38" t="n">
         <v>284</v>
       </c>
     </row>
@@ -25949,10 +25955,10 @@
       <c r="B41" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="C41" s="36" t="n">
+      <c r="C41" s="37" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="37" t="n">
+      <c r="D41" s="38" t="n">
         <v>300</v>
       </c>
     </row>
@@ -25963,10 +25969,10 @@
       <c r="B42" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="C42" s="36" t="n">
+      <c r="C42" s="37" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="37" t="n">
+      <c r="D42" s="38" t="n">
         <v>316</v>
       </c>
     </row>
@@ -25977,10 +25983,10 @@
       <c r="B43" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C43" s="36" t="n">
+      <c r="C43" s="37" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="36" t="n">
+      <c r="D43" s="37" t="n">
         <v>207</v>
       </c>
     </row>
@@ -25991,10 +25997,10 @@
       <c r="B44" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C44" s="36" t="n">
+      <c r="C44" s="37" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="36" t="n">
+      <c r="D44" s="37" t="n">
         <v>223</v>
       </c>
     </row>
@@ -26005,10 +26011,10 @@
       <c r="B45" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C45" s="36" t="n">
+      <c r="C45" s="37" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="37" t="n">
+      <c r="D45" s="38" t="n">
         <v>239</v>
       </c>
     </row>
@@ -26019,10 +26025,10 @@
       <c r="B46" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C46" s="36" t="n">
+      <c r="C46" s="37" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="36" t="n">
+      <c r="D46" s="37" t="n">
         <v>255</v>
       </c>
     </row>
@@ -26033,10 +26039,10 @@
       <c r="B47" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C47" s="36" t="n">
+      <c r="C47" s="37" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="37" t="n">
+      <c r="D47" s="38" t="n">
         <v>271</v>
       </c>
     </row>
@@ -26047,10 +26053,10 @@
       <c r="B48" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C48" s="36" t="n">
+      <c r="C48" s="37" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="37" t="n">
+      <c r="D48" s="38" t="n">
         <v>287</v>
       </c>
     </row>
@@ -26061,10 +26067,10 @@
       <c r="B49" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C49" s="36" t="n">
+      <c r="C49" s="37" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="37" t="n">
+      <c r="D49" s="38" t="n">
         <v>303</v>
       </c>
     </row>
@@ -26075,10 +26081,10 @@
       <c r="B50" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C50" s="36" t="n">
+      <c r="C50" s="37" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="37" t="n">
+      <c r="D50" s="38" t="n">
         <v>319</v>
       </c>
     </row>
@@ -27050,7 +27056,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -27062,32 +27068,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>928</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="40" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>929</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>